<commit_message>
Dp on String LC- 1092,1312,583
Dp on String LC- 1092,1312,583
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on String/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on String/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on String\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066F47F4-63C1-444F-B76F-D24C13E5E1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8591350-4CA0-41CC-89D4-A1C21316AA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Question No</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Longest Common Subsequence</t>
   </si>
   <si>
-    <t>Java</t>
-  </si>
-  <si>
     <t>Longest Palindromic Subsequence</t>
   </si>
   <si>
@@ -70,6 +67,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Java code</t>
+  </si>
+  <si>
+    <t>Minimum Insertion Steps to Make a String Palindrome</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Delete Operation for Two Strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">space optimization --&gt;LCS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortest Common Supersequence </t>
   </si>
 </sst>
 </file>
@@ -446,7 +461,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -502,67 +517,99 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1312</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>583</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="4">
+        <v>1092</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Leetcode 115,44,72 (recurssion,Memoization,tabulation,space optimization)
Leetcode 115,44,72 (recurssion,Memoization,tabulation,space optimization)
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on String/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on String/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on String\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8591350-4CA0-41CC-89D4-A1C21316AA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C882FF8-1073-4AD4-BCE8-C03D62EF2C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Question No</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t xml:space="preserve">Shortest Common Supersequence </t>
+  </si>
+  <si>
+    <t>Distinct Subsequences</t>
+  </si>
+  <si>
+    <t>Recurssion+Memoization+tabulation+space optimization</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>Wildcard Matching</t>
   </si>
 </sst>
 </file>
@@ -149,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -178,6 +190,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +476,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +485,7 @@
     <col min="2" max="2" width="20.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="43.140625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -612,26 +627,56 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>115</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="4">
+        <v>72</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="4">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>

</xml_diff>

<commit_message>
718. Maximum Length of Repeated Subarray
718. Maximum Length of Repeated Subarray
</commit_message>
<xml_diff>
--- a/Dynamic Programming/DP on String/Question_List-Java version.xlsx
+++ b/Dynamic Programming/DP on String/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\DP on String\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C882FF8-1073-4AD4-BCE8-C03D62EF2C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46DADC5-52CC-4AC5-A0E7-97E3FAA6FDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Question No</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Wildcard Matching</t>
+  </si>
+  <si>
+    <t>Maximum Length of Repeated Subarray</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -191,6 +200,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -476,7 +495,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,20 +560,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -678,11 +697,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>718</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>

</xml_diff>